<commit_message>
Updated INS datasets page function
</commit_message>
<xml_diff>
--- a/InputFiles/C3DC/TC01_C3DC_phs000463_SexAtBirth-Female.xlsx
+++ b/InputFiles/C3DC/TC01_C3DC_phs000463_SexAtBirth-Female.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sohilz2/Automation/05-01-2025/Commons_Automation/InputFiles/C3DC/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sohilz2/Automation/05-29-2025/Commons_Automation/InputFiles/C3DC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A0909DA-28A4-F44D-A14F-338CAFE41ECF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8ED6581-EA0F-AE48-8A28-0FBCADE459A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="35840" yWindow="-2240" windowWidth="30240" windowHeight="24500" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -290,7 +290,7 @@
 WHERE 
     std.dbgap_accession = 'phs000463' AND prt.sex_at_birth = 'Female' AND srv.survival_id IS NOT NULL
 ORDER BY 
-    prt.participant_id ASC
+   prt.participant_id ASC
 LIMIT 100;</t>
   </si>
 </sst>
@@ -298,9 +298,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -353,11 +360,14 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -683,8 +693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -769,7 +779,7 @@
       <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C7" s="2"/>
@@ -782,7 +792,7 @@
       <c r="C9" s="1"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated queries for C3DC first half testcases.
</commit_message>
<xml_diff>
--- a/InputFiles/C3DC/TC01_C3DC_phs000463_SexAtBirth-Female.xlsx
+++ b/InputFiles/C3DC/TC01_C3DC_phs000463_SexAtBirth-Female.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sohilz2/Automation/05-29-2025/Commons_Automation/InputFiles/C3DC/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sohilz2/Automation/07-15-2025/Commons_Automation/InputFiles/C3DC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8ED6581-EA0F-AE48-8A28-0FBCADE459A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBC268BD-AA96-B74A-9DCF-941D7059EF0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="35840" yWindow="-2240" windowWidth="30240" windowHeight="24500" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -84,17 +84,17 @@
 FROM 
     df_study std
 LEFT JOIN 
-    df_participant prt ON std.id = prt."study.id"
-LEFT JOIN 
-    df_diagnoses dgn ON prt.id = dgn."participant.id"
-LEFT JOIN 
-    df_treatments trt ON prt.id = trt."participant.id"
-LEFT JOIN 
-    df_treatment_resp trr ON prt.id = trr."participant.id"
-LEFT JOIN 
-    df_survival srv ON prt.id = srv."participant.id"
-LEFT JOIN 
-    df_reference_files rfs ON std.id = rfs."study.id"
+    df_participant prt ON std.study_id = prt."study.study_id"
+LEFT JOIN 
+    df_diagnoses dgn ON prt.participant_id = dgn."participant.participant_id"
+LEFT JOIN 
+    df_treatments trt ON prt.participant_id = trt."participant.participant_id"
+LEFT JOIN 
+    df_treatment_resp trr ON prt.participant_id = trr."participant.participant_id"
+LEFT JOIN 
+    df_survival srv ON prt.participant_id = srv."participant.participant_id"
+LEFT JOIN 
+    df_reference_files rfs ON std.study_id = rfs."study.study_id"
 WHERE 
    std.dbgap_accession = 'phs000463' AND prt.sex_at_birth = 'Female';</t>
   </si>
@@ -105,17 +105,17 @@
 FROM 
     df_study std
 LEFT JOIN 
-    df_participant prt ON std.id = prt."study.id"
-LEFT JOIN 
-    df_diagnoses dgn ON prt.id = dgn."participant.id"
-LEFT JOIN 
-    df_treatments trt ON prt.id = trt."participant.id"
-LEFT JOIN 
-    df_treatment_resp trr ON prt.id = trr."participant.id"
-LEFT JOIN 
-    df_survival srv ON prt.id = srv."participant.id"
-LEFT JOIN 
-    df_reference_files rfs ON std.id = rfs."study.id"
+    df_participant prt ON std.study_id = prt."study.study_id"
+LEFT JOIN 
+    df_diagnoses dgn ON prt.participant_id = dgn."participant.participant_id"
+LEFT JOIN 
+    df_treatments trt ON prt.participant_id = trt."participant.participant_id"
+LEFT JOIN 
+    df_treatment_resp trr ON prt.participant_id = trr."participant.participant_id"
+LEFT JOIN 
+    df_survival srv ON prt.participant_id = srv."participant.participant_id"
+LEFT JOIN 
+    df_reference_files rfs ON std.study_id = rfs."study.study_id"
 WHERE 
     std.dbgap_accession = 'phs000463' AND prt.sex_at_birth = 'Female'</t>
   </si>
@@ -128,17 +128,17 @@
 FROM 
     df_study std
 LEFT JOIN 
-    df_participant prt ON std.id = prt."study.id"
-LEFT JOIN 
-    df_diagnoses dgn ON prt.id = dgn."participant.id"
-LEFT JOIN 
-    df_treatments trt ON prt.id = trt."participant.id"
-LEFT JOIN 
-    df_treatment_resp trr ON prt.id = trr."participant.id"
-LEFT JOIN 
-    df_survival srv ON prt.id = srv."participant.id"
-LEFT JOIN 
-    df_reference_files rfs ON std.id = rfs."study.id"
+    df_participant prt ON std.study_id = prt."study.study_id"
+LEFT JOIN 
+    df_diagnoses dgn ON prt.participant_id = dgn."participant.participant_id"
+LEFT JOIN 
+    df_treatments trt ON prt.participant_id = trt."participant.participant_id"
+LEFT JOIN 
+    df_treatment_resp trr ON prt.participant_id = trr."participant.participant_id"
+LEFT JOIN 
+    df_survival srv ON prt.participant_id = srv."participant.participant_id"
+LEFT JOIN 
+    df_reference_files rfs ON std.study_id = rfs."study.study_id"
 WHERE 
     std.dbgap_accession = 'phs000463' AND prt.sex_at_birth = 'Female'
 ORDER BY 
@@ -165,17 +165,17 @@
 FROM 
     df_study std
 LEFT JOIN 
-    df_participant prt ON std.id = prt."study.id"
-LEFT JOIN 
-    df_diagnoses dgn ON prt.id = dgn."participant.id"
-LEFT JOIN 
-    df_treatments trt ON prt.id = trt."participant.id"
-LEFT JOIN 
-    df_treatment_resp trr ON prt.id = trr."participant.id"
-LEFT JOIN 
-    df_survival srv ON prt.id = srv."participant.id"
-LEFT JOIN 
-    df_reference_files rfs ON std.id = rfs."study.id"
+    df_participant prt ON std.study_id = prt."study.study_id"
+LEFT JOIN 
+    df_diagnoses dgn ON prt.participant_id = dgn."participant.participant_id"
+LEFT JOIN 
+    df_treatments trt ON prt.participant_id = trt."participant.participant_id"
+LEFT JOIN 
+    df_treatment_resp trr ON prt.participant_id = trr."participant.participant_id"
+LEFT JOIN 
+    df_survival srv ON prt.participant_id = srv."participant.participant_id"
+LEFT JOIN 
+    df_reference_files rfs ON std.study_id = rfs."study.study_id"
 WHERE 
     std.dbgap_accession = 'phs000463' AND prt.sex_at_birth = 'Female' AND dgn.diagnosis_id IS NOT NULL
 ORDER BY 
@@ -206,17 +206,17 @@
 FROM 
     df_study std
 LEFT JOIN 
-    df_participant prt ON std.id = prt."study.id"
-LEFT JOIN 
-    df_diagnoses dgn ON prt.id = dgn."participant.id"
-LEFT JOIN 
-    df_treatments trt ON prt.id = trt."participant.id"
-LEFT JOIN 
-    df_treatment_resp trr ON prt.id = trr."participant.id"
-LEFT JOIN 
-    df_survival srv ON prt.id = srv."participant.id"
-LEFT JOIN 
-    df_reference_files rfs ON std.id = rfs."study.id"
+    df_participant prt ON std.study_id = prt."study.study_id"
+LEFT JOIN 
+    df_diagnoses dgn ON prt.participant_id = dgn."participant.participant_id"
+LEFT JOIN 
+    df_treatments trt ON prt.participant_id = trt."participant.participant_id"
+LEFT JOIN 
+    df_treatment_resp trr ON prt.participant_id = trr."participant.participant_id"
+LEFT JOIN 
+    df_survival srv ON prt.participant_id = srv."participant.participant_id"
+LEFT JOIN 
+    df_reference_files rfs ON std.study_id = rfs."study.study_id"
 WHERE 
     std.dbgap_accession = 'phs000463' AND prt.sex_at_birth = 'Female'
 ORDER BY 
@@ -241,19 +241,17 @@
 FROM 
     df_study std
 LEFT JOIN 
-    df_participant prt ON std.id = prt."study.id"
-LEFT JOIN 
-    df_diagnoses dgn ON prt.id = dgn."participant.id"
-LEFT JOIN 
-    df_treatments trt ON prt.id = trt."participant.id"
-LEFT JOIN 
-    df_treatment_resp trr ON prt.id = trr."participant.id"
-LEFT JOIN 
-    df_survival srv ON prt.id = srv."participant.id"
-LEFT JOIN 
-    df_reference_files rfs ON std.id = rfs."study.id"
-WHERE 
-    std.dbgap_accession = 'phs000463' AND prt.sex_at_birth = 'Female'
+    df_participant prt ON std.study_id = prt."study.study_id"
+LEFT JOIN 
+    df_diagnoses dgn ON prt.participant_id = dgn."participant.participant_id"
+LEFT JOIN 
+    df_treatments trt ON prt.participant_id = trt."participant.participant_id"
+LEFT JOIN 
+    df_treatment_resp trr ON prt.participant_id = trr."participant.participant_id"
+LEFT JOIN 
+    df_survival srv ON prt.participant_id = srv."participant.participant_id"
+LEFT JOIN 
+    df_reference_files rfs ON std.study_id = rfs."study.study_id"
 ORDER BY 
     prt.participant_id ASC
 LIMIT 100;</t>
@@ -276,17 +274,17 @@
 FROM 
     df_study std
 LEFT JOIN 
-    df_participant prt ON std.id = prt."study.id"
-LEFT JOIN 
-    df_diagnoses dgn ON prt.id = dgn."participant.id"
-LEFT JOIN 
-    df_treatments trt ON prt.id = trt."participant.id"
-LEFT JOIN 
-    df_treatment_resp trr ON prt.id = trr."participant.id"
-LEFT JOIN 
-    df_survival srv ON prt.id = srv."participant.id"
-LEFT JOIN 
-    df_reference_files rfs ON std.id = rfs."study.id"
+    df_participant prt ON std.study_id = prt."study.study_id"
+LEFT JOIN 
+    df_diagnoses dgn ON prt.participant_id = dgn."participant.participant_id"
+LEFT JOIN 
+    df_treatments trt ON prt.participant_id = trt."participant.participant_id"
+LEFT JOIN 
+    df_treatment_resp trr ON prt.participant_id = trr."participant.participant_id"
+LEFT JOIN 
+    df_survival srv ON prt.participant_id = srv."participant.participant_id"
+LEFT JOIN 
+    df_reference_files rfs ON std.study_id = rfs."study.study_id"
 WHERE 
     std.dbgap_accession = 'phs000463' AND prt.sex_at_birth = 'Female' AND srv.survival_id IS NOT NULL
 ORDER BY 
@@ -298,16 +296,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -360,14 +351,11 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -693,7 +681,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -779,7 +767,7 @@
       <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C7" s="2"/>
@@ -792,7 +780,7 @@
       <c r="C9" s="1"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added CTDC sample testcase for filter sex
</commit_message>
<xml_diff>
--- a/InputFiles/C3DC/TC01_C3DC_phs000463_SexAtBirth-Female.xlsx
+++ b/InputFiles/C3DC/TC01_C3DC_phs000463_SexAtBirth-Female.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11018"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sohilz2/Automation/07-15-2025/Commons_Automation/InputFiles/C3DC/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sohilz2/Automation/10-23-2025/Commons_Automation/InputFiles/C3DC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBC268BD-AA96-B74A-9DCF-941D7059EF0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ADD4393-E765-A943-8D71-1414464885EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35840" yWindow="-2240" windowWidth="30240" windowHeight="24500" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="-41480" yWindow="-1100" windowWidth="30240" windowHeight="24500" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -77,68 +77,58 @@
     <t>TC01_C3DC_phs000463_SexAtBirth-Female_TSVData.xlsx</t>
   </si>
   <si>
-    <t>SELECT 
-    COUNT(DISTINCT dgn.diagnosis) AS Diagnoses,
-    COUNT(DISTINCT prt.participant_id) AS Participants,
-    COUNT(DISTINCT std.study_id) AS Studies
-FROM 
-    df_study std
-LEFT JOIN 
-    df_participant prt ON std.study_id = prt."study.study_id"
-LEFT JOIN 
-    df_diagnoses dgn ON prt.participant_id = dgn."participant.participant_id"
-LEFT JOIN 
-    df_treatments trt ON prt.participant_id = trt."participant.participant_id"
-LEFT JOIN 
-    df_treatment_resp trr ON prt.participant_id = trr."participant.participant_id"
-LEFT JOIN 
-    df_survival srv ON prt.participant_id = srv."participant.participant_id"
-LEFT JOIN 
-    df_reference_files rfs ON std.study_id = rfs."study.study_id"
-WHERE 
-   std.dbgap_accession = 'phs000463' AND prt.sex_at_birth = 'Female';</t>
-  </si>
-  <si>
     <t>SELECT DISTINCT
      std.dbgap_accession AS "dbGaP Accession",
      std.study_name AS "Study Name"
 FROM 
     df_study std
 LEFT JOIN 
-    df_participant prt ON std.study_id = prt."study.study_id"
-LEFT JOIN 
-    df_diagnoses dgn ON prt.participant_id = dgn."participant.participant_id"
-LEFT JOIN 
-    df_treatments trt ON prt.participant_id = trt."participant.participant_id"
-LEFT JOIN 
-    df_treatment_resp trr ON prt.participant_id = trr."participant.participant_id"
-LEFT JOIN 
-    df_survival srv ON prt.participant_id = srv."participant.participant_id"
-LEFT JOIN 
-    df_reference_files rfs ON std.study_id = rfs."study.study_id"
-WHERE 
-    std.dbgap_accession = 'phs000463' AND prt.sex_at_birth = 'Female'</t>
+    df_participant prt 
+        ON 1=1   -- participants not directly linked to studies
+LEFT JOIN 
+    df_diagnoses dgn 
+        ON prt.id = dgn."participant.id"
+LEFT JOIN 
+    df_treatments trt 
+        ON prt.id = trt."participant.id"
+LEFT JOIN 
+    df_treatment_resp trr 
+        ON prt.id = trr."participant.id"
+LEFT JOIN 
+    df_survival srv 
+        ON prt.id = srv."participant.id"
+LEFT JOIN 
+    df_genetic_analyses ga 
+        ON prt.id = ga."participant.id"
+WHERE  
+    std.dbgap_accession = 'phs000463' AND prt.sex_at_birth = 'Female';</t>
   </si>
   <si>
     <t>SELECT DISTINCT
     prt.participant_id AS "Participant Id",
-    prt.race AS "Race",
+    REPLACE(prt.race, ';', ', ') AS "Race",
     prt.sex_at_birth AS "Sex at Birth",
     std.dbgap_accession AS "dbGaP Accession"
 FROM 
     df_study std
 LEFT JOIN 
-    df_participant prt ON std.study_id = prt."study.study_id"
-LEFT JOIN 
-    df_diagnoses dgn ON prt.participant_id = dgn."participant.participant_id"
-LEFT JOIN 
-    df_treatments trt ON prt.participant_id = trt."participant.participant_id"
-LEFT JOIN 
-    df_treatment_resp trr ON prt.participant_id = trr."participant.participant_id"
-LEFT JOIN 
-    df_survival srv ON prt.participant_id = srv."participant.participant_id"
-LEFT JOIN 
-    df_reference_files rfs ON std.study_id = rfs."study.study_id"
+    df_participant prt 
+        ON 1=1   -- participants not directly linked to studies
+LEFT JOIN 
+    df_diagnoses dgn 
+        ON prt.id = dgn."participant.id"
+LEFT JOIN 
+    df_treatments trt 
+        ON prt.id = trt."participant.id"
+LEFT JOIN 
+    df_treatment_resp trr 
+        ON prt.id = trr."participant.id"
+LEFT JOIN 
+    df_survival srv 
+        ON prt.id = srv."participant.id"
+LEFT JOIN 
+    df_genetic_analyses ga 
+        ON prt.id = ga."participant.id"
 WHERE 
     std.dbgap_accession = 'phs000463' AND prt.sex_at_birth = 'Female'
 ORDER BY 
@@ -165,21 +155,27 @@
 FROM 
     df_study std
 LEFT JOIN 
-    df_participant prt ON std.study_id = prt."study.study_id"
-LEFT JOIN 
-    df_diagnoses dgn ON prt.participant_id = dgn."participant.participant_id"
-LEFT JOIN 
-    df_treatments trt ON prt.participant_id = trt."participant.participant_id"
-LEFT JOIN 
-    df_treatment_resp trr ON prt.participant_id = trr."participant.participant_id"
-LEFT JOIN 
-    df_survival srv ON prt.participant_id = srv."participant.participant_id"
-LEFT JOIN 
-    df_reference_files rfs ON std.study_id = rfs."study.study_id"
+    df_participant prt 
+        ON 1=1   -- participants not directly linked to studies
+LEFT JOIN 
+    df_diagnoses dgn 
+        ON prt.id = dgn."participant.id"
+LEFT JOIN 
+    df_treatments trt 
+        ON prt.id = trt."participant.id"
+LEFT JOIN 
+    df_treatment_resp trr 
+        ON prt.id = trr."participant.id"
+LEFT JOIN 
+    df_survival srv 
+        ON prt.id = srv."participant.id"
+LEFT JOIN 
+    df_genetic_analyses ga 
+        ON prt.id = ga."participant.id"
 WHERE 
     std.dbgap_accession = 'phs000463' AND prt.sex_at_birth = 'Female' AND dgn.diagnosis_id IS NOT NULL
 ORDER BY 
-    prt.participant_id ASC
+    CAST(prt.participant_id AS TEXT) ASC
 LIMIT 100;</t>
   </si>
   <si>
@@ -206,22 +202,50 @@
 FROM 
     df_study std
 LEFT JOIN 
-    df_participant prt ON std.study_id = prt."study.study_id"
-LEFT JOIN 
-    df_diagnoses dgn ON prt.participant_id = dgn."participant.participant_id"
-LEFT JOIN 
-    df_treatments trt ON prt.participant_id = trt."participant.participant_id"
-LEFT JOIN 
-    df_treatment_resp trr ON prt.participant_id = trr."participant.participant_id"
-LEFT JOIN 
-    df_survival srv ON prt.participant_id = srv."participant.participant_id"
-LEFT JOIN 
-    df_reference_files rfs ON std.study_id = rfs."study.study_id"
-WHERE 
+    df_participant prt 
+        ON 1=1   -- participants not directly linked to studies
+LEFT JOIN 
+    df_diagnoses dgn 
+        ON prt.id = dgn."participant.id"
+LEFT JOIN 
+    df_treatments trt 
+        ON prt.id = trt."participant.id"
+LEFT JOIN 
+    df_treatment_resp trr 
+        ON prt.id = trr."participant.id"
+LEFT JOIN 
+    df_survival srv 
+        ON prt.id = srv."participant.id"
+LEFT JOIN 
+    df_genetic_analyses ga 
+        ON prt.id = ga."participant.id"
+WHERE  
     std.dbgap_accession = 'phs000463' AND prt.sex_at_birth = 'Female'
 ORDER BY 
     trt.treatment_id ASC
 LIMIT 100;</t>
+  </si>
+  <si>
+    <t>SELECT 
+    COUNT(DISTINCT dgn.diagnosis) AS Diagnoses,
+    COUNT(DISTINCT prt.participant_id) AS Participants,
+    COUNT(DISTINCT std.study_id) AS Studies
+FROM 
+    df_study std
+LEFT JOIN 
+    df_participant prt ON 1=1   -- participants not directly linked to studies
+LEFT JOIN 
+    df_diagnoses dgn ON prt.id = dgn."participant.id"
+LEFT JOIN 
+    df_treatments trt ON prt.id = trt."participant.id"
+LEFT JOIN 
+    df_treatment_resp trr ON prt.id = trr."participant.id"
+LEFT JOIN 
+    df_survival srv ON prt.id = srv."participant.id"
+LEFT JOIN 
+    df_genetic_analyses ga ON prt.id = ga."participant.id"
+WHERE     
+    std.dbgap_accession = 'phs000463' AND prt.sex_at_birth = 'Female';</t>
   </si>
   <si>
     <t>SELECT DISTINCT
@@ -241,17 +265,20 @@
 FROM 
     df_study std
 LEFT JOIN 
-    df_participant prt ON std.study_id = prt."study.study_id"
-LEFT JOIN 
-    df_diagnoses dgn ON prt.participant_id = dgn."participant.participant_id"
-LEFT JOIN 
-    df_treatments trt ON prt.participant_id = trt."participant.participant_id"
-LEFT JOIN 
-    df_treatment_resp trr ON prt.participant_id = trr."participant.participant_id"
-LEFT JOIN 
-    df_survival srv ON prt.participant_id = srv."participant.participant_id"
-LEFT JOIN 
-    df_reference_files rfs ON std.study_id = rfs."study.study_id"
+    df_participant prt 
+        ON 1=1   -- participants not directly linked to studies
+LEFT JOIN 
+    df_diagnoses dgn ON prt.id = dgn."participant.id"
+LEFT JOIN 
+    df_treatments trt ON prt.id = trt."participant.id"
+LEFT JOIN 
+    df_treatment_resp trr ON prt.id = trr."participant.id"
+LEFT JOIN 
+    df_survival srv ON prt.id = srv."participant.id"
+LEFT JOIN 
+    df_genetic_analyses ga ON prt.id = ga."participant.id"
+WHERE
+    std.dbgap_accession = 'phs000463' AND prt.sex_at_birth = 'Female' 
 ORDER BY 
     prt.participant_id ASC
 LIMIT 100;</t>
@@ -274,18 +301,18 @@
 FROM 
     df_study std
 LEFT JOIN 
-    df_participant prt ON std.study_id = prt."study.study_id"
-LEFT JOIN 
-    df_diagnoses dgn ON prt.participant_id = dgn."participant.participant_id"
-LEFT JOIN 
-    df_treatments trt ON prt.participant_id = trt."participant.participant_id"
-LEFT JOIN 
-    df_treatment_resp trr ON prt.participant_id = trr."participant.participant_id"
-LEFT JOIN 
-    df_survival srv ON prt.participant_id = srv."participant.participant_id"
-LEFT JOIN 
-    df_reference_files rfs ON std.study_id = rfs."study.study_id"
-WHERE 
+    df_participant prt ON 1=1   -- participants not directly linked to studies
+LEFT JOIN 
+    df_diagnoses dgn ON prt.id = dgn."participant.id"
+LEFT JOIN 
+    df_treatments trt ON prt.id = trt."participant.id"
+LEFT JOIN 
+    df_treatment_resp trr ON prt.id = trr."participant.id"
+LEFT JOIN 
+    df_survival srv ON prt.id = srv."participant.id"
+LEFT JOIN 
+    df_genetic_analyses ga ON prt.id = ga."participant.id"
+WHERE
     std.dbgap_accession = 'phs000463' AND prt.sex_at_birth = 'Female' AND srv.survival_id IS NOT NULL
 ORDER BY 
    prt.participant_id ASC
@@ -716,10 +743,10 @@
         <v>8</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
         <v>12</v>
@@ -733,7 +760,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
@@ -741,7 +768,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4" s="2"/>
     </row>
@@ -750,7 +777,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" s="2"/>
     </row>

</xml_diff>